<commit_message>
Another 3 tests are added
</commit_message>
<xml_diff>
--- a/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
+++ b/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B826D5-D00E-D34C-B304-D288AC1024F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B842E9F8-FE9C-3942-8793-7907B5ADA445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="4160" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7520" yWindow="3860" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="30">
   <si>
     <t>Feature 1</t>
   </si>
@@ -330,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -435,6 +435,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -719,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,6 +983,21 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
+      <c r="F10" s="28">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="G10" s="28">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
@@ -993,6 +1011,21 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
+      <c r="F11" s="28">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="18" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
@@ -1006,10 +1039,21 @@
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+      <c r="F12" s="36">
+        <v>0.37152777777777779</v>
+      </c>
+      <c r="G12" s="36">
+        <v>0.37430555555555556</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
@@ -1177,8 +1221,12 @@
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="F23" s="27">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="G23" s="27">
+        <v>0.63749999999999996</v>
+      </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
     </row>
@@ -1194,6 +1242,12 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
+      <c r="F24" s="28">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="G24" s="28">
+        <v>0.65763888888888888</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
@@ -1207,6 +1261,12 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
+      <c r="F25" s="28">
+        <v>0.67777777777777781</v>
+      </c>
+      <c r="G25" s="28">
+        <v>0.6791666666666667</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">

</xml_diff>

<commit_message>
Functional Testing Assignment: Gherkin files are added
</commit_message>
<xml_diff>
--- a/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
+++ b/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B842E9F8-FE9C-3942-8793-7907B5ADA445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00436AE9-7E6B-1A47-87F1-A752E8BFBA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7520" yWindow="3860" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="33">
   <si>
     <t>Feature 1</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>Correct: The generate code was correct.</t>
+  </si>
+  <si>
+    <t>The same problem as the feature 1 has occurred that is solved. I've solved the problem with using Thread.sleep(2000);</t>
+  </si>
+  <si>
+    <t>I've solved the problem with using Thread.sleep(2000);</t>
+  </si>
+  <si>
+    <t>STOP Development Time</t>
   </si>
 </sst>
 </file>
@@ -359,9 +368,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,9 +380,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -395,9 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,6 +416,15 @@
     <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,7 +446,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -722,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J560"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -771,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
@@ -787,36 +796,36 @@
       </c>
       <c r="J2" s="32"/>
     </row>
-    <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24">
         <v>0.37777777777777777</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="24">
         <v>0.38055555555555554</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -827,21 +836,21 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="28">
+      <c r="F4" s="25">
         <v>0.38194444444444442</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="25">
         <v>0.38750000000000001</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="25">
         <v>0.55347222222222225</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="25">
         <v>0.55486111111111114</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -852,21 +861,21 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="28">
+      <c r="F5" s="25">
         <v>0.38819444444444445</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="25">
         <v>0.39097222222222222</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="25">
         <v>0.55555555555555558</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="25">
         <v>0.55625000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -877,16 +886,16 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="28">
+      <c r="F6" s="25">
         <v>0.3923611111111111</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="25">
         <v>0.39791666666666664</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="25" t="s">
         <v>28</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -894,7 +903,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -905,16 +914,16 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="28">
+      <c r="F7" s="25">
         <v>0.39861111111111114</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="25">
         <v>0.40138888888888891</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="25" t="s">
         <v>28</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -922,7 +931,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -933,21 +942,21 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="28">
+      <c r="F8" s="25">
         <v>0.40208333333333335</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="25">
         <v>0.40625</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="25">
         <v>0.55763888888888891</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="25">
         <v>0.55833333333333335</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -958,21 +967,21 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="28">
+      <c r="F9" s="25">
         <v>0.4284722222222222</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="25">
         <v>0.43263888888888891</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="25">
         <v>0.55833333333333335</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="25">
         <v>0.56736111111111109</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -983,10 +992,10 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="28">
+      <c r="F10" s="25">
         <v>0.35694444444444445</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="25">
         <v>0.3576388888888889</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -1000,7 +1009,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1011,10 +1020,10 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="28">
+      <c r="F11" s="25">
         <v>0.36388888888888887</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="25">
         <v>0.3659722222222222</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -1027,31 +1036,31 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:10" s="16" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="36">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="26">
         <v>0.37152777777777779</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="26">
         <v>0.37430555555555556</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1065,12 +1074,16 @@
       <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="D13" s="27">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.69236111111111109</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1081,6 +1094,12 @@
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D14" s="28">
+        <v>0.69652777777777775</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0.71250000000000002</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1097,6 +1116,12 @@
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D15" s="28">
+        <v>0.76944444444444449</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0.77222222222222225</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1112,12 +1137,18 @@
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D16" s="28">
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0.3576388888888889</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -1126,13 +1157,19 @@
       </c>
       <c r="C17" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D17" s="28">
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="E17" s="28">
+        <v>0.37361111111111112</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1141,13 +1178,19 @@
       </c>
       <c r="C18" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D18" s="28">
+        <v>0.37569444444444444</v>
+      </c>
+      <c r="E18" s="28">
+        <v>0.37777777777777777</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1156,13 +1199,19 @@
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D19" s="28">
+        <v>0.38124999999999998</v>
+      </c>
+      <c r="E19" s="28">
+        <v>0.3972222222222222</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1171,13 +1220,19 @@
       </c>
       <c r="C20" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D20" s="28">
+        <v>0.40138888888888891</v>
+      </c>
+      <c r="E20" s="28">
+        <v>0.40277777777777779</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1186,52 +1241,69 @@
       </c>
       <c r="C21" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D21" s="28">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="E21" s="28">
+        <v>0.42083333333333334</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" s="21" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+    <row r="22" spans="1:10" s="19" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-    </row>
-    <row r="23" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="D22" s="36">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E22" s="36">
+        <v>0.43472222222222223</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="27">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="24">
         <v>0.62916666666666665</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="24">
         <v>0.63749999999999996</v>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="H23" s="24">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I23" s="24">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1242,15 +1314,24 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="28">
+      <c r="F24" s="25">
         <v>0.64930555555555558</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="25">
         <v>0.65763888888888888</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="H24" s="25">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="I24" s="25">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1261,15 +1342,24 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="28">
+      <c r="F25" s="25">
         <v>0.67777777777777781</v>
       </c>
-      <c r="G25" s="28">
+      <c r="G25" s="25">
         <v>0.6791666666666667</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="H25" s="25">
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="I25" s="25">
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1280,9 +1370,24 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="F26" s="25">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G26" s="25">
+        <v>0.41944444444444445</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1293,9 +1398,24 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="F27" s="25">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="G27" s="25">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1306,9 +1426,24 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="F28" s="25">
+        <v>0.44513888888888886</v>
+      </c>
+      <c r="G28" s="25">
+        <v>0.44722222222222224</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1319,9 +1454,24 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+      <c r="F29" s="25">
+        <v>0.45277777777777778</v>
+      </c>
+      <c r="G29" s="25">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1332,9 +1482,24 @@
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="F30" s="25">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G30" s="25">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1345,43 +1510,45 @@
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:9" s="18" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" spans="1:10" s="16" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1396,7 +1563,7 @@
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1411,7 +1578,7 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1426,7 +1593,7 @@
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1441,7 +1608,7 @@
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1456,7 +1623,7 @@
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1471,7 +1638,7 @@
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1486,7 +1653,7 @@
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1500,22 +1667,22 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" s="18" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+    <row r="42" spans="1:9" s="16" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Project is updated + Excel file is updated
</commit_message>
<xml_diff>
--- a/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
+++ b/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00436AE9-7E6B-1A47-87F1-A752E8BFBA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A40357-159C-3841-BCB0-9CC4505E8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="3860" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4220" yWindow="3060" windowWidth="23620" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,12 +401,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -425,6 +419,18 @@
     <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,9 +450,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -731,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -747,22 +750,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="31" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33" t="s">
         <v>22</v>
       </c>
     </row>
@@ -794,7 +797,7 @@
       <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="32"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -806,22 +809,19 @@
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24">
-        <v>0.37777777777777777</v>
-      </c>
-      <c r="G3" s="24">
-        <v>0.38055555555555554</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>29</v>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22">
+        <v>0.4375</v>
+      </c>
+      <c r="G3" s="22">
+        <v>0.44236111111111109</v>
+      </c>
+      <c r="H3" s="22">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="I3" s="22">
+        <v>0.68541666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -836,17 +836,20 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="25">
-        <v>0.38194444444444442</v>
-      </c>
-      <c r="G4" s="25">
-        <v>0.38750000000000001</v>
-      </c>
-      <c r="H4" s="25">
-        <v>0.55347222222222225</v>
-      </c>
-      <c r="I4" s="25">
-        <v>0.55486111111111114</v>
+      <c r="F4" s="23">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -861,17 +864,20 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="25">
-        <v>0.38819444444444445</v>
-      </c>
-      <c r="G5" s="25">
-        <v>0.39097222222222222</v>
-      </c>
-      <c r="H5" s="25">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="I5" s="25">
-        <v>0.55625000000000002</v>
+      <c r="F5" s="23">
+        <v>0.59791666666666665</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -886,16 +892,16 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="25">
-        <v>0.3923611111111111</v>
-      </c>
-      <c r="G6" s="25">
-        <v>0.39791666666666664</v>
-      </c>
-      <c r="H6" s="25" t="s">
+      <c r="F6" s="23">
+        <v>0.60138888888888886</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.60486111111111107</v>
+      </c>
+      <c r="H6" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="23" t="s">
         <v>28</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -914,20 +920,17 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="25">
-        <v>0.39861111111111114</v>
-      </c>
-      <c r="G7" s="25">
-        <v>0.40138888888888891</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>29</v>
+      <c r="F7" s="23">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.60763888888888884</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0.68611111111111112</v>
+      </c>
+      <c r="I7" s="23">
+        <v>0.68611111111111112</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -942,17 +945,20 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="25">
-        <v>0.40208333333333335</v>
-      </c>
-      <c r="G8" s="25">
-        <v>0.40625</v>
-      </c>
-      <c r="H8" s="25">
-        <v>0.55763888888888891</v>
-      </c>
-      <c r="I8" s="25">
-        <v>0.55833333333333335</v>
+      <c r="F8" s="23">
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.61388888888888893</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -967,17 +973,17 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="25">
-        <v>0.4284722222222222</v>
-      </c>
-      <c r="G9" s="25">
-        <v>0.43263888888888891</v>
-      </c>
-      <c r="H9" s="25">
-        <v>0.55833333333333335</v>
-      </c>
-      <c r="I9" s="25">
-        <v>0.56736111111111109</v>
+      <c r="F9" s="23">
+        <v>0.6381944444444444</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0.6875</v>
+      </c>
+      <c r="I9" s="23">
+        <v>0.68958333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -992,11 +998,11 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="25">
-        <v>0.35694444444444445</v>
-      </c>
-      <c r="G10" s="25">
-        <v>0.3576388888888889</v>
+      <c r="F10" s="23">
+        <v>0.64652777777777781</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.65138888888888891</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>28</v>
@@ -1020,20 +1026,17 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="25">
-        <v>0.36388888888888887</v>
-      </c>
-      <c r="G11" s="25">
-        <v>0.3659722222222222</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>29</v>
+      <c r="F11" s="23">
+        <v>0.65208333333333335</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="H11" s="23">
+        <v>0.68680555555555556</v>
+      </c>
+      <c r="I11" s="23">
+        <v>0.68680555555555556</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="16" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1048,11 +1051,11 @@
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="26">
-        <v>0.37152777777777779</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0.37430555555555556</v>
+      <c r="F12" s="24">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0.65902777777777777</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>28</v>
@@ -1074,10 +1077,10 @@
       <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="25">
         <v>0.68125000000000002</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="25">
         <v>0.69236111111111109</v>
       </c>
       <c r="F13" s="10"/>
@@ -1095,10 +1098,10 @@
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="26">
         <v>0.69652777777777775</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="26">
         <v>0.71250000000000002</v>
       </c>
       <c r="F14" s="6"/>
@@ -1116,10 +1119,10 @@
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="26">
         <v>0.76944444444444449</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="26">
         <v>0.77222222222222225</v>
       </c>
       <c r="F15" s="6"/>
@@ -1137,10 +1140,10 @@
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="26">
         <v>0.35486111111111113</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <v>0.3576388888888889</v>
       </c>
       <c r="F16" s="6"/>
@@ -1158,10 +1161,10 @@
       <c r="C17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="26">
         <v>0.35902777777777778</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="26">
         <v>0.37361111111111112</v>
       </c>
       <c r="F17" s="6"/>
@@ -1179,10 +1182,10 @@
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="26">
         <v>0.37569444444444444</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="26">
         <v>0.37777777777777777</v>
       </c>
       <c r="F18" s="6"/>
@@ -1200,10 +1203,10 @@
       <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="26">
         <v>0.38124999999999998</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="26">
         <v>0.3972222222222222</v>
       </c>
       <c r="F19" s="6"/>
@@ -1221,10 +1224,10 @@
       <c r="C20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="26">
         <v>0.40138888888888891</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="26">
         <v>0.40277777777777779</v>
       </c>
       <c r="F20" s="6"/>
@@ -1242,10 +1245,10 @@
       <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="26">
         <v>0.40555555555555556</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="26">
         <v>0.42083333333333334</v>
       </c>
       <c r="F21" s="6"/>
@@ -1263,10 +1266,10 @@
       <c r="C22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="27">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="27">
         <v>0.43472222222222223</v>
       </c>
       <c r="F22" s="20"/>
@@ -1286,16 +1289,16 @@
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="F23" s="24">
+      <c r="F23" s="22">
         <v>0.62916666666666665</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="22">
         <v>0.63749999999999996</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="22">
         <v>0.58333333333333337</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I23" s="22">
         <v>0.6166666666666667</v>
       </c>
       <c r="J23" s="12" t="s">
@@ -1314,16 +1317,16 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="25">
+      <c r="F24" s="23">
         <v>0.64930555555555558</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="23">
         <v>0.65763888888888888</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="23">
         <v>0.6166666666666667</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="23">
         <v>0.6166666666666667</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -1342,16 +1345,16 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="25">
+      <c r="F25" s="23">
         <v>0.67777777777777781</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="23">
         <v>0.6791666666666667</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="23">
         <v>0.62222222222222223</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="23">
         <v>0.62222222222222223</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -1370,10 +1373,10 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="25">
+      <c r="F26" s="23">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="23">
         <v>0.41944444444444445</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -1398,10 +1401,10 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="25">
+      <c r="F27" s="23">
         <v>0.42291666666666666</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="23">
         <v>0.42569444444444443</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -1426,10 +1429,10 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
-      <c r="F28" s="25">
+      <c r="F28" s="23">
         <v>0.44513888888888886</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="23">
         <v>0.44722222222222224</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -1454,10 +1457,10 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="25">
+      <c r="F29" s="23">
         <v>0.45277777777777778</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="23">
         <v>0.45555555555555555</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -1482,10 +1485,10 @@
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
-      <c r="F30" s="25">
+      <c r="F30" s="23">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="23">
         <v>0.4597222222222222</v>
       </c>
       <c r="H30" s="4" t="s">
@@ -1510,8 +1513,8 @@
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:10" s="16" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
@@ -1525,8 +1528,8 @@
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
     </row>
@@ -1540,8 +1543,12 @@
       <c r="C33" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="D33" s="28">
+        <v>0.65</v>
+      </c>
+      <c r="E33" s="28">
+        <v>0.67500000000000004</v>
+      </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
@@ -1557,6 +1564,12 @@
       <c r="C34" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D34" s="26">
+        <v>0.7319444444444444</v>
+      </c>
+      <c r="E34" s="26">
+        <v>0.74444444444444446</v>
+      </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -1572,6 +1585,12 @@
       <c r="C35" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D35" s="26">
+        <v>0.74861111111111112</v>
+      </c>
+      <c r="E35" s="26">
+        <v>0.75138888888888888</v>
+      </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -1587,6 +1606,12 @@
       <c r="C36" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D36" s="26">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="E36" s="26">
+        <v>0.42638888888888887</v>
+      </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -1602,6 +1627,12 @@
       <c r="C37" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D37" s="26">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="E37" s="26">
+        <v>0.43263888888888891</v>
+      </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -1617,6 +1648,12 @@
       <c r="C38" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D38" s="26">
+        <v>0.4375</v>
+      </c>
+      <c r="E38" s="26">
+        <v>0.44305555555555554</v>
+      </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -1632,6 +1669,12 @@
       <c r="C39" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D39" s="26">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E39" s="26">
+        <v>0.46388888888888891</v>
+      </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -1647,6 +1690,12 @@
       <c r="C40" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D40" s="26">
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="E40" s="26">
+        <v>0.47291666666666665</v>
+      </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -1662,6 +1711,12 @@
       <c r="C41" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D41" s="26">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E41" s="26">
+        <v>0.56874999999999998</v>
+      </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -1677,14 +1732,21 @@
       <c r="C42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
+      <c r="D42" s="29">
+        <v>0.58611111111111114</v>
+      </c>
+      <c r="E42" s="29">
+        <v>0.6381944444444444</v>
+      </c>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+    </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>

</xml_diff>

<commit_message>
All Projects' Tests are implemented + Excel file is updated
</commit_message>
<xml_diff>
--- a/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
+++ b/Functional Part/Assignment/ASSESSOR+ Time Sheet - Group A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A40357-159C-3841-BCB0-9CC4505E8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AF8B81-066F-8A40-B371-912E50673310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="3060" windowWidth="23620" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="1700" windowWidth="23620" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="31">
   <si>
     <t>Feature 1</t>
   </si>
@@ -110,12 +110,6 @@
   </si>
   <si>
     <t>Correct: The generate code was correct.</t>
-  </si>
-  <si>
-    <t>The same problem as the feature 1 has occurred that is solved. I've solved the problem with using Thread.sleep(2000);</t>
-  </si>
-  <si>
-    <t>I've solved the problem with using Thread.sleep(2000);</t>
   </si>
   <si>
     <t>STOP Development Time</t>
@@ -735,7 +729,7 @@
   <dimension ref="A1:J560"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -783,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
@@ -1290,19 +1284,16 @@
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="22">
-        <v>0.62916666666666665</v>
+        <v>0.7368055555555556</v>
       </c>
       <c r="G23" s="22">
-        <v>0.63749999999999996</v>
+        <v>0.74027777777777781</v>
       </c>
       <c r="H23" s="22">
-        <v>0.58333333333333337</v>
+        <v>0.48680555555555555</v>
       </c>
       <c r="I23" s="22">
-        <v>0.6166666666666667</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>31</v>
+        <v>0.48749999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1318,19 +1309,16 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="23">
-        <v>0.64930555555555558</v>
+        <v>0.74097222222222225</v>
       </c>
       <c r="G24" s="23">
-        <v>0.65763888888888888</v>
+        <v>0.74513888888888891</v>
       </c>
       <c r="H24" s="23">
-        <v>0.6166666666666667</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="I24" s="23">
-        <v>0.6166666666666667</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>30</v>
+        <v>0.48888888888888887</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1346,19 +1334,16 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="23">
-        <v>0.67777777777777781</v>
+        <v>0.74583333333333335</v>
       </c>
       <c r="G25" s="23">
-        <v>0.6791666666666667</v>
+        <v>0.74930555555555556</v>
       </c>
       <c r="H25" s="23">
-        <v>0.62222222222222223</v>
+        <v>0.49236111111111114</v>
       </c>
       <c r="I25" s="23">
-        <v>0.62222222222222223</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>30</v>
+        <v>0.49583333333333335</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1374,10 +1359,10 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="23">
-        <v>0.41666666666666669</v>
+        <v>0.75</v>
       </c>
       <c r="G26" s="23">
-        <v>0.41944444444444445</v>
+        <v>0.75416666666666665</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>28</v>
@@ -1402,10 +1387,10 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="23">
-        <v>0.42291666666666666</v>
+        <v>0.75486111111111109</v>
       </c>
       <c r="G27" s="23">
-        <v>0.42569444444444443</v>
+        <v>0.75694444444444442</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>28</v>
@@ -1430,10 +1415,10 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="23">
-        <v>0.44513888888888886</v>
+        <v>0.45763888888888887</v>
       </c>
       <c r="G28" s="23">
-        <v>0.44722222222222224</v>
+        <v>0.46111111111111114</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>28</v>
@@ -1458,19 +1443,16 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="23">
-        <v>0.45277777777777778</v>
+        <v>0.46458333333333335</v>
       </c>
       <c r="G29" s="23">
-        <v>0.45555555555555555</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>29</v>
+        <v>0.46597222222222223</v>
+      </c>
+      <c r="H29" s="23">
+        <v>0.49930555555555556</v>
+      </c>
+      <c r="I29" s="23">
+        <v>0.50972222222222219</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1486,10 +1468,10 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="23">
-        <v>0.45833333333333331</v>
+        <v>0.76458333333333328</v>
       </c>
       <c r="G30" s="23">
-        <v>0.4597222222222222</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>28</v>
@@ -1513,8 +1495,21 @@
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="F31" s="23">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="G31" s="23">
+        <v>0.76944444444444449</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:10" s="16" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
@@ -1528,10 +1523,21 @@
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="F32" s="24">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G32" s="24">
+        <v>0.7729166666666667</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="33" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">

</xml_diff>